<commit_message>
Commit 2 - updated code
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishal.nandy\Documents\NC Quiz Tool Demo\Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6376FB-EB27-4A6B-9CC6-E6264862ED7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696A61D1-B103-46C5-B5B7-F61561221D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,21 +42,6 @@
     <t>Chennai</t>
   </si>
   <si>
-    <t>q1</t>
-  </si>
-  <si>
-    <t>q2</t>
-  </si>
-  <si>
-    <t>q3</t>
-  </si>
-  <si>
-    <t>q4</t>
-  </si>
-  <si>
-    <t>Questions</t>
-  </si>
-  <si>
     <t>Correct Answer</t>
   </si>
   <si>
@@ -103,6 +88,21 @@
   </si>
   <si>
     <t>Kazan</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>Option A</t>
+  </si>
+  <si>
+    <t>Option B</t>
+  </si>
+  <si>
+    <t>Option C</t>
+  </si>
+  <si>
+    <t>Option D</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -435,22 +435,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -475,62 +475,62 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit 4 - updated code
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishal.nandy\Documents\NC Quiz Tool Demo\Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696A61D1-B103-46C5-B5B7-F61561221D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52ABAC9C-7039-455F-A6F7-C8535EFB8C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,22 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
-  <si>
-    <t>What is the capital of India?</t>
-  </si>
-  <si>
-    <t>Kolkata</t>
-  </si>
-  <si>
-    <t>New Delhi</t>
-  </si>
-  <si>
-    <t>Mumbai</t>
-  </si>
-  <si>
-    <t>Chennai</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Correct Answer</t>
   </si>
@@ -103,19 +88,43 @@
   </si>
   <si>
     <t>Option D</t>
+  </si>
+  <si>
+    <t>Which all NC's are under-Sketch Sheets: Provide the details of surrounding fasteners installed or holes drilled.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bent </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dent </t>
+  </si>
+  <si>
+    <t>Wanted Hole</t>
+  </si>
+  <si>
+    <t>All the above</t>
+  </si>
+  <si>
+    <t>Dent, Bent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -126,7 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -134,12 +143,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="dotted">
+        <color auto="1"/>
+      </left>
+      <right style="dotted">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,114 +450,114 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="93.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>